<commit_message>
Updating gnps mgf function
</commit_message>
<xml_diff>
--- a/inst/extdata/GNPS_template.xlsx
+++ b/inst/extdata/GNPS_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirozmoreno.1/Documents/GitHub/MS2extract/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D22F7D6-5A70-2044-894F-79B09DADF9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E523F0-CA46-444E-A6E8-542D78EF7B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37240" yWindow="560" windowWidth="38420" windowHeight="20380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37240" yWindow="560" windowWidth="38420" windowHeight="20380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GNSP Template" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>FILENAME</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>DanielitoQuiroz</t>
+  </si>
+  <si>
+    <t>20 eV</t>
   </si>
 </sst>
 </file>
@@ -684,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDE0C25-F82B-9D4C-B0BD-24F9B19B59DE}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -882,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03095276-8950-3A46-9C03-13871663E218}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -894,7 +897,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>'GNSP Template'!C1</f>
         <v>COMPOUND_NAME</v>
@@ -967,15 +970,15 @@
         <v>PI</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1">
-        <v>20</v>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>40</v>
@@ -1023,15 +1026,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1">
-        <v>20</v>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Updating mgf write for GNPS format
</commit_message>
<xml_diff>
--- a/inst/extdata/GNPS_template.xlsx
+++ b/inst/extdata/GNPS_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirozmoreno.1/Documents/GitHub/MS2extract/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9EDC62-FA76-D746-9951-75A7E7CCE15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5D708C-D1CF-E142-8603-776B1882B21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38420" yWindow="560" windowWidth="38420" windowHeight="20380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35160" yWindow="500" windowWidth="28580" windowHeight="15560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GNSP Template" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
   <si>
     <t>FILENAME</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>20 eV</t>
+  </si>
+  <si>
+    <t>LC-ESI</t>
   </si>
 </sst>
 </file>
@@ -232,9 +235,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -519,7 +521,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -687,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDE0C25-F82B-9D4C-B0BD-24F9B19B59DE}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="173" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -800,10 +802,10 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
@@ -812,7 +814,7 @@
       <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F2" t="s">
@@ -821,7 +823,7 @@
       <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I2" t="s">
@@ -833,7 +835,7 @@
       <c r="K2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M2" t="s">
@@ -845,13 +847,13 @@
       <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q2" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="S2" t="s">
@@ -885,202 +887,199 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03095276-8950-3A46-9C03-13871663E218}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
-    <col min="6" max="10" width="10.83203125" style="1"/>
-    <col min="11" max="11" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
+      <c r="A1" t="str">
         <f>'GNSP Template'!C1</f>
         <v>COMPOUND_NAME</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <f>'GNSP Template'!E1</f>
         <v>INSTRUMENT</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" t="str">
         <f>'GNSP Template'!F1</f>
         <v>IONSOURCE</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="E1" t="str">
         <f>'GNSP Template'!H1</f>
         <v>SMILES</v>
       </c>
-      <c r="F1" s="1" t="str">
+      <c r="F1" t="str">
         <f>'GNSP Template'!I1</f>
         <v>INCHI</v>
       </c>
-      <c r="G1" s="1" t="str">
+      <c r="G1" t="str">
         <f>'GNSP Template'!J1</f>
         <v>INCHIAUX</v>
       </c>
-      <c r="H1" s="1" t="str">
+      <c r="H1" t="str">
         <f>'GNSP Template'!L1</f>
         <v>IONMODE</v>
       </c>
-      <c r="I1" s="1" t="str">
+      <c r="I1" t="str">
         <f>'GNSP Template'!M1</f>
         <v>PUBMED</v>
       </c>
-      <c r="J1" s="1" t="str">
+      <c r="J1" t="str">
         <f>'GNSP Template'!N1</f>
         <v>ACQUISITION</v>
       </c>
-      <c r="K1" s="1" t="str">
+      <c r="K1" t="str">
         <f>'GNSP Template'!P1</f>
         <v>DATACOLLECTOR</v>
       </c>
-      <c r="L1" s="1" t="str">
+      <c r="L1" t="str">
         <f>'GNSP Template'!R1</f>
         <v>INTEREST</v>
       </c>
-      <c r="M1" s="1" t="str">
+      <c r="M1" t="str">
         <f>'GNSP Template'!S1</f>
         <v>LIBQUALITY</v>
       </c>
-      <c r="N1" s="1" t="str">
+      <c r="N1" t="str">
         <f>'GNSP Template'!T1</f>
         <v>GENUS</v>
       </c>
-      <c r="O1" s="1" t="str">
+      <c r="O1" t="str">
         <f>'GNSP Template'!U1</f>
         <v>SPECIES</v>
       </c>
-      <c r="P1" s="1" t="str">
+      <c r="P1" t="str">
         <f>'GNSP Template'!V1</f>
         <v>STRAIN</v>
       </c>
-      <c r="Q1" s="1" t="str">
+      <c r="Q1" t="str">
         <f>'GNSP Template'!W1</f>
         <v>CASNUMBER</v>
       </c>
-      <c r="R1" s="1" t="str">
+      <c r="R1" t="str">
         <f>'GNSP Template'!X1</f>
         <v>PI</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3">
         <v>2</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding feature GNPS export
</commit_message>
<xml_diff>
--- a/inst/extdata/GNPS_template.xlsx
+++ b/inst/extdata/GNPS_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirozmoreno.1/Documents/GitHub/MS2extract/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5D708C-D1CF-E142-8603-776B1882B21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C16EA9-AA4E-4240-AB7F-0B06BA730525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35160" yWindow="500" windowWidth="28580" windowHeight="15560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37800" yWindow="13880" windowWidth="27040" windowHeight="6600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GNSP Template" sheetId="1" r:id="rId1"/>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -689,13 +689,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDE0C25-F82B-9D4C-B0BD-24F9B19B59DE}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -887,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03095276-8950-3A46-9C03-13871663E218}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>